<commit_message>
add sheet names to output, indent work done on tab
</commit_message>
<xml_diff>
--- a/Tests/multiple tabs - different.xlsx
+++ b/Tests/multiple tabs - different.xlsx
@@ -1,33 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\spreadsheet-comparison-tool\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D77746FB-40D5-43D0-8E78-006A653BF172}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B011DC-9E86-4F6C-81ED-FB99B8FB3519}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{968A31B8-81EC-499F-B8EF-0F3E2CA58A8A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{968A31B8-81EC-499F-B8EF-0F3E2CA58A8A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="namedTab1" sheetId="1" r:id="rId1"/>
+    <sheet name="namedTab2" sheetId="2" r:id="rId2"/>
+    <sheet name="namedTab3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>10,16</t>
   </si>
@@ -4638,7 +4643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4D1BAE-F3E7-455A-BA1E-93B9BF15BD89}">
   <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
@@ -8859,8 +8864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E28AF56-0EEE-47E3-8EB9-6EAD59F0D53D}">
   <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA35" sqref="AA35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8981,7 +8986,7 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f t="shared" ref="A2:P37" si="1">(ROW()-1)*28+COLUMN()</f>
+        <f t="shared" ref="A2:P26" si="1">(ROW()-1)*28+COLUMN()</f>
         <v>29</v>
       </c>
       <c r="B2">
@@ -9939,7 +9944,7 @@
         <v>265</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10:AB37" si="2">(ROW()-1)*28+COLUMN()</f>
+        <f t="shared" ref="N10:AB35" si="2">(ROW()-1)*28+COLUMN()</f>
         <v>266</v>
       </c>
       <c r="O10">

</xml_diff>